<commit_message>
Built database framework; did migrations; added StudyApp.Model to the repository.
</commit_message>
<xml_diff>
--- a/Design/Database/Logical Table Representation.xlsx
+++ b/Design/Database/Logical Table Representation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewmoore/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewmoore/Documents/Computer Programming/MSSA/Coding/Project/study-project/Design/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEBAE793-C5FB-0144-AA94-E73A3CACB50E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED250427-B79C-3E49-871A-1BD9C79F11D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{11D4F990-D8BF-464E-AF05-E525BBAC729E}"/>
+    <workbookView xWindow="7680" yWindow="-16600" windowWidth="28040" windowHeight="17040" xr2:uid="{11D4F990-D8BF-464E-AF05-E525BBAC729E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Users</t>
   </si>
@@ -42,55 +42,85 @@
     <t>Subjects</t>
   </si>
   <si>
-    <t>Defintions</t>
-  </si>
-  <si>
     <t>Difficulty Level</t>
   </si>
   <si>
     <t>Reminders</t>
   </si>
   <si>
-    <t>Study Scores</t>
-  </si>
-  <si>
-    <t>Forgetting Rate</t>
-  </si>
-  <si>
-    <t>Emails</t>
-  </si>
-  <si>
-    <t>Usernames</t>
-  </si>
-  <si>
     <t>Answers</t>
   </si>
   <si>
-    <t>Contact Info</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>Correct Answers</t>
-  </si>
-  <si>
     <t>Values</t>
   </si>
   <si>
-    <t>Times</t>
-  </si>
-  <si>
     <t>Study Score</t>
   </si>
   <si>
-    <t>userid</t>
-  </si>
-  <si>
-    <t>Incorrect Answers</t>
-  </si>
-  <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>TermId</t>
+  </si>
+  <si>
+    <t>SubejectId</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>SubjectId</t>
+  </si>
+  <si>
+    <t>ForgettingRate</t>
+  </si>
+  <si>
+    <t>UserNames</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>DefinitionId</t>
+  </si>
+  <si>
+    <t>CorrectAns</t>
+  </si>
+  <si>
+    <t>IncorrectAns</t>
+  </si>
+  <si>
+    <t>AnswerId</t>
+  </si>
+  <si>
+    <t>QuestionId</t>
+  </si>
+  <si>
+    <t>DateCorrect</t>
+  </si>
+  <si>
+    <t>TimeTaken</t>
+  </si>
+  <si>
+    <t>Ans</t>
+  </si>
+  <si>
+    <t>DateReviewed</t>
+  </si>
+  <si>
+    <t>Qs</t>
+  </si>
+  <si>
+    <t>Defs</t>
+  </si>
+  <si>
+    <t>TermNames</t>
+  </si>
+  <si>
+    <t>SubjectNames</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
   </si>
 </sst>
 </file>
@@ -147,7 +177,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9E93AB90-2587-E84E-9378-604F5B43568F}" name="Table2" displayName="Table2" ref="C1:C11" totalsRowShown="0">
-  <autoFilter ref="C1:C11" xr:uid="{50E1DE69-1E7F-B24B-9D8A-FF734286A5EB}"/>
+  <autoFilter ref="C1:C11" xr:uid="{50E1DE69-1E7F-B24B-9D8A-FF734286A5EB}">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{90CE233C-32B5-AA4B-944D-F90117B73F1C}" name="Users"/>
   </tableColumns>
@@ -156,16 +192,6 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F0D9C6E0-20BA-2441-8743-A230CCF199C4}" name="Table3" displayName="Table3" ref="A1:A4" totalsRowShown="0">
-  <autoFilter ref="A1:A4" xr:uid="{192F6D6D-1609-4B4F-99E1-156EB7CD16D9}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{F389484F-86AC-6E40-8B6A-525647C4C6F5}" name="Contact Info"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C4A39051-8C27-CC49-A890-FA0BA5B970A2}" name="Table4" displayName="Table4" ref="E1:E5" totalsRowShown="0">
   <autoFilter ref="E1:E5" xr:uid="{ABFA5D5E-F377-FF42-A33C-0857E6558BBA}"/>
   <tableColumns count="1">
@@ -175,9 +201,15 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B95B069D-9ECE-3440-ABE2-90BE45F58F9D}" name="Table5" displayName="Table5" ref="C13:C19" totalsRowShown="0">
-  <autoFilter ref="C13:C19" xr:uid="{6E987EB5-B95B-9641-8FBB-1E70686FB130}"/>
+  <autoFilter ref="C13:C19" xr:uid="{6E987EB5-B95B-9641-8FBB-1E70686FB130}">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{608D005A-08C1-3D4B-A74A-91FDC3611244}" name="Terms"/>
   </tableColumns>
@@ -185,9 +217,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{89728609-9340-4D42-9B11-1B4116ADFECA}" name="Table6" displayName="Table6" ref="A14:A17" totalsRowShown="0">
-  <autoFilter ref="A14:A17" xr:uid="{ADC515C7-4772-784D-B4DE-E61A874667B5}"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{89728609-9340-4D42-9B11-1B4116ADFECA}" name="Table6" displayName="Table6" ref="A14:A19" totalsRowShown="0">
+  <autoFilter ref="A14:A19" xr:uid="{ADC515C7-4772-784D-B4DE-E61A874667B5}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{2B3D816C-D84D-D64D-8537-C41EFAE55C68}" name="Subjects"/>
   </tableColumns>
@@ -195,9 +227,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{65AFA7F3-FD1D-A346-BB2E-92BF96F8CAC1}" name="Table7" displayName="Table7" ref="E14:E18" totalsRowShown="0">
-  <autoFilter ref="E14:E18" xr:uid="{3BEF83DC-5587-674F-A402-42C5A54AB8AA}"/>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{65AFA7F3-FD1D-A346-BB2E-92BF96F8CAC1}" name="Table7" displayName="Table7" ref="E14:E20" totalsRowShown="0">
+  <autoFilter ref="E14:E20" xr:uid="{3BEF83DC-5587-674F-A402-42C5A54AB8AA}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{6D7C7E4E-F87F-1B49-A783-A7D6A7F74AA6}" name="Definitions"/>
   </tableColumns>
@@ -205,9 +237,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{62CA9043-0805-A944-8458-1591C5C3CD68}" name="Table8" displayName="Table8" ref="E21:E23" totalsRowShown="0">
-  <autoFilter ref="E21:E23" xr:uid="{9B4D2E9D-5BC6-6646-9E9E-4197074CC498}"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{62CA9043-0805-A944-8458-1591C5C3CD68}" name="Table8" displayName="Table8" ref="E22:E26" totalsRowShown="0">
+  <autoFilter ref="E22:E26" xr:uid="{9B4D2E9D-5BC6-6646-9E9E-4197074CC498}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{09D6B94B-4444-C245-8B63-A513801A309A}" name="Questions"/>
   </tableColumns>
@@ -215,9 +247,15 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{40F0FD3F-E22B-E74C-AFDB-2C3C6A37C706}" name="Table10" displayName="Table10" ref="E25:E27" totalsRowShown="0">
-  <autoFilter ref="E25:E27" xr:uid="{DBD584ED-C96F-6946-9D05-3F53B65A12A6}"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{40F0FD3F-E22B-E74C-AFDB-2C3C6A37C706}" name="Table10" displayName="Table10" ref="E28:E36" totalsRowShown="0">
+  <autoFilter ref="E28:E36" xr:uid="{DBD584ED-C96F-6946-9D05-3F53B65A12A6}">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{E1142852-E147-9E46-9F82-974400083BCB}" name="Answers"/>
   </tableColumns>
@@ -522,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7CCE0E2-2D87-F541-9D40-EADE78D714B4}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C19"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -537,87 +575,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-    </row>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>1</v>
@@ -628,7 +638,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
         <v>2</v>
@@ -636,78 +646,127 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E21" t="s">
-        <v>3</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E22" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E23" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E25" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E26" t="s">
-        <v>16</v>
-      </c>
-    </row>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" hidden="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="8">
+  <tableParts count="7">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -715,7 +774,6 @@
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
-    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>